<commit_message>
Power of Attorney code so far
</commit_message>
<xml_diff>
--- a/Data_File/GeneralPOA.xlsx
+++ b/Data_File/GeneralPOA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AB0215E\OneDrive - Absa\My Documents\April\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEEF500-051E-47FD-8810-C279961503BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8697E8B-8A3D-42C3-9D07-EAD67C4B61A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="2460" windowWidth="21600" windowHeight="11385" xr2:uid="{3CC51130-3266-47B1-A7A3-BCAA268D1A7B}"/>
+    <workbookView xWindow="2670" yWindow="3765" windowWidth="21600" windowHeight="11385" xr2:uid="{3CC51130-3266-47B1-A7A3-BCAA268D1A7B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>Username</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>MORROW</t>
-  </si>
-  <si>
-    <t>01</t>
   </si>
   <si>
     <t>T</t>
@@ -213,12 +210,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -536,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC85FB8B-6AF0-4CE6-9D48-50E007754314}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +610,7 @@
         <v>20</v>
       </c>
       <c r="R1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="S1" t="s">
         <v>21</v>
@@ -664,17 +662,17 @@
       <c r="E2">
         <v>4048644149</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>34</v>
+      <c r="F2" s="5">
+        <v>2</v>
       </c>
       <c r="G2">
         <v>888</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="5">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
         <v>34</v>
-      </c>
-      <c r="I2" t="s">
-        <v>35</v>
       </c>
       <c r="J2">
         <v>12121985</v>
@@ -686,10 +684,10 @@
         <v>32</v>
       </c>
       <c r="N2" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="O2" s="5">
+        <v>1</v>
       </c>
       <c r="P2" s="2">
         <v>8512120097080</v>
@@ -698,40 +696,40 @@
         <v>11042022</v>
       </c>
       <c r="R2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
         <v>37</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" s="5">
+        <v>1</v>
+      </c>
+      <c r="V2" s="5">
+        <v>1</v>
+      </c>
+      <c r="W2" s="5">
+        <v>1</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="U2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="AA2">
         <v>3100</v>
       </c>
       <c r="AB2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC2" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="AC2" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>